<commit_message>
backup befpre category implementation
</commit_message>
<xml_diff>
--- a/price.xlsx
+++ b/price.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -559,7 +559,18 @@
         <v>11</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>45233.68721516226</v>
+        <v>45233.68721516203</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>9</v>
+      </c>
+      <c r="B12" t="n">
+        <v>255</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>45234.50345805833</v>
       </c>
     </row>
   </sheetData>

</xml_diff>